<commit_message>
Update InterviewQuestions (Core Java).xlsx
</commit_message>
<xml_diff>
--- a/src/com/corejava/practice/topics/InterviewQuestions (Core Java).xlsx
+++ b/src/com/corejava/practice/topics/InterviewQuestions (Core Java).xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="106">
   <si>
     <t>Topic</t>
   </si>
@@ -320,6 +320,21 @@
   </si>
   <si>
     <t>https://github.com/palarghya337/CoreJava/blob/master/src/com/corejava/practice/multithreading/SemaphoreExample.java</t>
+  </si>
+  <si>
+    <t>When to use LinkedList over ArrayList?</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/322715/when-to-use-linkedlist-over-arraylist-in-java?rq=1</t>
+  </si>
+  <si>
+    <t>When static variable is loaded in java?</t>
+  </si>
+  <si>
+    <t>Memory Management</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/4343760/when-is-static-variable-loaded-in-java-runtime-or-compile-time</t>
   </si>
 </sst>
 </file>
@@ -1194,11 +1209,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C69"/>
+  <dimension ref="A1:C71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C69" sqref="C69"/>
+      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A83" sqref="A83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1869,6 +1884,28 @@
       </c>
       <c r="C69" s="3" t="s">
         <v>100</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="30">
+      <c r="A70" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="30">
+      <c r="A71" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -1890,8 +1927,10 @@
     <hyperlink ref="C58" r:id="rId11"/>
     <hyperlink ref="C63" r:id="rId12"/>
     <hyperlink ref="C69" r:id="rId13"/>
+    <hyperlink ref="C70" r:id="rId14"/>
+    <hyperlink ref="C71" r:id="rId15"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId14"/>
+  <pageSetup orientation="portrait" r:id="rId16"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Expand to se more
• Updated the code and added comments for CountDownLatchExample and CyclicBarrierExample
• Added new interview question.
</commit_message>
<xml_diff>
--- a/src/com/corejava/practice/topics/InterviewQuestions (Core Java).xlsx
+++ b/src/com/corejava/practice/topics/InterviewQuestions (Core Java).xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="107">
   <si>
     <t>Topic</t>
   </si>
@@ -304,9 +304,6 @@
     <t>Java8</t>
   </si>
   <si>
-    <t>What is flatmap?</t>
-  </si>
-  <si>
     <t>Static variables belong to a class and not to any individual instance. The concept of serialization is concerned with the object's current state. Only data associated with a specific instance of a class is serialized, therefore static member fields are ignored during serialization.</t>
   </si>
   <si>
@@ -335,6 +332,12 @@
   </si>
   <si>
     <t>https://stackoverflow.com/questions/4343760/when-is-static-variable-loaded-in-java-runtime-or-compile-time</t>
+  </si>
+  <si>
+    <t>What is the difference between map() and flatMap()?</t>
+  </si>
+  <si>
+    <t>https://javarevisited.blogspot.com/2016/03/difference-between-map-and-flatmap-in-java8.html</t>
   </si>
 </sst>
 </file>
@@ -1212,8 +1215,8 @@
   <dimension ref="A1:C71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A83" sqref="A83"/>
+      <pane ySplit="1" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1505,7 +1508,7 @@
         <v>41</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -1850,21 +1853,23 @@
       </c>
       <c r="C65" s="2"/>
     </row>
-    <row r="66" spans="1:3">
+    <row r="66" spans="1:3" ht="30">
       <c r="A66" s="2" t="s">
         <v>94</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="C66" s="2"/>
+        <v>105</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -1872,7 +1877,7 @@
         <v>24</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="45">
@@ -1880,10 +1885,10 @@
         <v>24</v>
       </c>
       <c r="B69" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C69" s="3" t="s">
         <v>99</v>
-      </c>
-      <c r="C69" s="3" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="30">
@@ -1891,21 +1896,21 @@
         <v>27</v>
       </c>
       <c r="B70" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C70" s="3" t="s">
         <v>101</v>
-      </c>
-      <c r="C70" s="3" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="30">
       <c r="A71" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C71" s="3" t="s">
         <v>104</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="C71" s="3" t="s">
-        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -1929,8 +1934,9 @@
     <hyperlink ref="C69" r:id="rId13"/>
     <hyperlink ref="C70" r:id="rId14"/>
     <hyperlink ref="C71" r:id="rId15"/>
+    <hyperlink ref="C66" r:id="rId16"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId16"/>
+  <pageSetup orientation="portrait" r:id="rId17"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Expand to see the details.
• Added example for flatMap() method of stream api.
• Added more interview questions.
• Added toString() method in WithoutComparableImplementation class.
• Added example for single vs parallel streaming
• how to find the nth largest element using stream api.
</commit_message>
<xml_diff>
--- a/src/com/corejava/practice/topics/InterviewQuestions (Core Java).xlsx
+++ b/src/com/corejava/practice/topics/InterviewQuestions (Core Java).xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="113">
   <si>
     <t>Topic</t>
   </si>
@@ -338,6 +338,24 @@
   </si>
   <si>
     <t>https://javarevisited.blogspot.com/2016/03/difference-between-map-and-flatmap-in-java8.html</t>
+  </si>
+  <si>
+    <t>What is Stream in Java 8?</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/stream-in-java/</t>
+  </si>
+  <si>
+    <t>How to sort a list of Object?</t>
+  </si>
+  <si>
+    <t>What is WeakHashMap?</t>
+  </si>
+  <si>
+    <t>What is the difference between stream() and parallelStream()?</t>
+  </si>
+  <si>
+    <t>https://www.developer.com/java/data/what-are-sequential-vs.-parallel-streams-in-java.html</t>
   </si>
 </sst>
 </file>
@@ -854,7 +872,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -868,6 +886,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1212,11 +1231,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C71"/>
+  <dimension ref="A1:C75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B66" sqref="B66"/>
+      <pane ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B79" sqref="B79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1911,6 +1930,44 @@
       </c>
       <c r="C71" s="3" t="s">
         <v>104</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C72" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" ht="30">
+      <c r="A75" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -1935,8 +1992,10 @@
     <hyperlink ref="C70" r:id="rId14"/>
     <hyperlink ref="C71" r:id="rId15"/>
     <hyperlink ref="C66" r:id="rId16"/>
+    <hyperlink ref="C72" r:id="rId17"/>
+    <hyperlink ref="C75" r:id="rId18"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId17"/>
+  <pageSetup orientation="portrait" r:id="rId19"/>
 </worksheet>
 </file>
</xml_diff>